<commit_message>
pr and rfq changes
</commit_message>
<xml_diff>
--- a/webroot/uploads/stock_upload_sample.xlsx
+++ b/webroot/uploads/stock_upload_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepaksingh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudee\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8508987F-5106-F342-8AF8-F69BAAD84954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C6BFE-2ACD-439D-BB3D-49CC188C5704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{631A87B2-296D-1E41-9317-1191F05A7849}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{631A87B2-296D-1E41-9317-1191F05A7849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,30 +20,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Current Stock</t>
   </si>
   <si>
-    <t>MAT_TEST</t>
-  </si>
-  <si>
-    <t>Mat Descriptions</t>
-  </si>
-  <si>
     <t>Part Code</t>
   </si>
   <si>
@@ -53,17 +39,17 @@
     <t>Part Desc</t>
   </si>
   <si>
-    <t>MAT_TEST2</t>
-  </si>
-  <si>
-    <t>Mat Descriptions2</t>
+    <t>489 UV/VIS DETECTOR 176002489 WATERS</t>
+  </si>
+  <si>
+    <t>SDPTEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,16 +57,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,12 +86,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,63 +419,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1EE70-9E11-9445-A137-C8808382E68A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
       <c r="D2">
         <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>122</v>
-      </c>
-      <c r="D3">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>